<commit_message>
📝 Actualizar datos hasta décimo encuentro
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Visualización_Caracterización_20240909.xlsx
+++ b/aplicaciones/procesador/datos/Visualización_Caracterización_20240909.xlsx
@@ -1,19 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enflujo\lab\unal-cuenco\aplicaciones\procesador\datos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE60879-F216-4B34-A1EE-594B9B1ABDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$H$246</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$246</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -23,926 +28,926 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="303">
-  <si>
-    <t xml:space="preserve">ENCUENTRO INTERSEDES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PERSONA PARTICIPANTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUGAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIPO DE SEDE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARGO O ÁREA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODIFICACIÓN POR TIPOLOGÍA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primer Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CECP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Bogotá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Andina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Docente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director Académico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BogSA-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director Instituto de Investigación en Educación (IIEDU)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AFMC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director Grupo de Investigación en Políticas Públicas de Educación Superior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEBT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director Dirección Nacional de Innovación Académica (DNIA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PFM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Manizales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MzlSA-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GHB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directora Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Palmira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PalSA-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WADA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Tumaco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede de Presencia Nacional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secretario de Sede</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TmcSP-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egresado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MzlSA-III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMGL</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="304">
+  <si>
+    <t>ENCUENTRO INTERSEDES</t>
+  </si>
+  <si>
+    <t>PERSONA PARTICIPANTE</t>
+  </si>
+  <si>
+    <t>LUGAR</t>
+  </si>
+  <si>
+    <t>TIPO DE SEDE</t>
+  </si>
+  <si>
+    <t>ROL</t>
+  </si>
+  <si>
+    <t>CARGO O ÁREA</t>
+  </si>
+  <si>
+    <t>CODIFICACIÓN POR TIPOLOGÍA</t>
+  </si>
+  <si>
+    <t>Primer Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>CECP</t>
+  </si>
+  <si>
+    <t>Sede Bogotá</t>
+  </si>
+  <si>
+    <t>Sede Andina</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
+    <t>Director Académico</t>
+  </si>
+  <si>
+    <t>BogSA-I</t>
+  </si>
+  <si>
+    <t>JCM</t>
+  </si>
+  <si>
+    <t>Director Instituto de Investigación en Educación (IIEDU)</t>
+  </si>
+  <si>
+    <t>AFMC</t>
+  </si>
+  <si>
+    <t>Director Grupo de Investigación en Políticas Públicas de Educación Superior</t>
+  </si>
+  <si>
+    <t>GEBT</t>
+  </si>
+  <si>
+    <t>Director Dirección Nacional de Innovación Académica (DNIA)</t>
+  </si>
+  <si>
+    <t>PFM</t>
+  </si>
+  <si>
+    <t>Sede Manizales</t>
+  </si>
+  <si>
+    <t>MzlSA-I</t>
+  </si>
+  <si>
+    <t>GHB</t>
+  </si>
+  <si>
+    <t>Directora Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>EDGL</t>
+  </si>
+  <si>
+    <t>Sede Palmira</t>
+  </si>
+  <si>
+    <t>PalSA-I</t>
+  </si>
+  <si>
+    <t>WADA</t>
+  </si>
+  <si>
+    <t>Sede Tumaco</t>
+  </si>
+  <si>
+    <t>Sede de Presencia Nacional</t>
+  </si>
+  <si>
+    <t>Secretario de Sede</t>
+  </si>
+  <si>
+    <t>TmcSP-I</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Egresado</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>MzlSA-III</t>
+  </si>
+  <si>
+    <t>DMGL</t>
   </si>
   <si>
     <t xml:space="preserve">Administrativo </t>
   </si>
   <si>
-    <t xml:space="preserve">Asistente Vicerrectoría Académica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BogSA-VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segundo Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vicerrector Académico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actor del territorio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neuropsicóloga y asesora organizacional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MzlSA-IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contratista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MzlSA-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tercer Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede de La Paz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DlaPSA-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Medellín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedSA-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASMR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudiante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representante PEAMA - PEAMA Orinoquía (Sede Origen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MzlSA-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KNH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Análisis de datos Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuarto Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JHC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equipo DNIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECMR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MdeSA-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decano Facultad de Ciencias Exactas y Naturales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KLB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directora Departamento de Matemáticas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director Académico Sede Palmira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCMR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Amazonía</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AmzSP-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HACM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JGCR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMMH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JDOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Caribe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrbSP-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede Orinoquía</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OrnSP-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JFGR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BogSA-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDVS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JFR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AmzSP-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asistente administrativa DNIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BogSA-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGRG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JPT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMMO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinadora funcional Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diseñadora visual Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asesora Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extensionista Facultad de Ciencias Exactas y Naturales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VJMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AmzSP-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMPM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Líder pedagógica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEBA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Líder de psicología</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JESB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quinto Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLRB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directora Departamento de Comunicación Humana Facultad de Medicina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AFOA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director CEMarin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directora Sede Caribe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DASC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RVM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grupo de investigación TecMarín</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SVO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maestría en Políticas Públicas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PVS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrbSP-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BBC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrbSP-III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NDG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KBG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artista raizal, participante proyecto El Otro Mar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrbSP-IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QBG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funcionario Corporación para el Desarrollo Sostenible del Archipiélago de San Andrés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funcionario Gobernación de San Andrés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KJR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PalSA-IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extensión Sede Caribe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrbSP-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FGP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinadora de la Unidad de Transformación Pedagógica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sexto Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JFRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maestría en Estudios Amazónicos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dirección Académica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMGC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unidad de Transformación Pedagógica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DLMG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CJQC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALRT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grupo de Apoyo Pedagógico Facultad de Medicina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCGN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrante Instituto de Estudios en Comunicación y Cultura (IECO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MABU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEAMA Orinoquía (Sede origen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMMV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centro Latinoamericano de Investigación e Innovación Científica (CLIIC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BogSA-VII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAVP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administrativo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supernumeraria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrbSP-VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sede De La Paz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intérprete Lengua de Señas Colombiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WAAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DGH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proyecto Política de Educación Inclusiva UNAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profesional de apoyo Política de Educación Inclusiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCRB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinador Acompañamiento Integral Bienestar Universitario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diseño web Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistematización de datos Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RARR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directora Bienestar Universitario Sede Manizales y Directora del proyecto Política de Educación Inclusiva UNAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vicerrector Sede Manizales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSLMR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEAMA Tumaco (Sede Origen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JSAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representante Estudiantil Consejo Académico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAMJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RHPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KAPJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEAMA Amazonía (Sede Origen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MdeSA-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistema de Acompañamiento Estudiantil Bienestar Universitario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PalSA-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MACA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEAMA Caribe (Sede Origen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PalSA-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JDHM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin identificar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA-VII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Séptimo Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRVM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrante Colectivo Cuerpos diversos en rebeldía</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EAER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KBV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrante Colectivo Cuerpos diversos en rebeldía
+    <t>Asistente Vicerrectoría Académica</t>
+  </si>
+  <si>
+    <t>BogSA-VI</t>
+  </si>
+  <si>
+    <t>Segundo Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>CAH</t>
+  </si>
+  <si>
+    <t>Vicerrector Académico</t>
+  </si>
+  <si>
+    <t>CMOS</t>
+  </si>
+  <si>
+    <t>Actor del territorio</t>
+  </si>
+  <si>
+    <t>Neuropsicóloga y asesora organizacional</t>
+  </si>
+  <si>
+    <t>MzlSA-IV</t>
+  </si>
+  <si>
+    <t>MCP</t>
+  </si>
+  <si>
+    <t>Contratista</t>
+  </si>
+  <si>
+    <t>Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>MzlSA-V</t>
+  </si>
+  <si>
+    <t>Tercer Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>JAP</t>
+  </si>
+  <si>
+    <t>Sede de La Paz</t>
+  </si>
+  <si>
+    <t>DlaPSA-I</t>
+  </si>
+  <si>
+    <t>JCOB</t>
+  </si>
+  <si>
+    <t>Sede Medellín</t>
+  </si>
+  <si>
+    <t>MedSA-I</t>
+  </si>
+  <si>
+    <t>ASMR</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
+    <t>Representante PEAMA - PEAMA Orinoquía (Sede Origen)</t>
+  </si>
+  <si>
+    <t>MzlSA-II</t>
+  </si>
+  <si>
+    <t>DEA</t>
+  </si>
+  <si>
+    <t>CLD</t>
+  </si>
+  <si>
+    <t>WAA</t>
+  </si>
+  <si>
+    <t>KNH</t>
+  </si>
+  <si>
+    <t>Análisis de datos Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>Cuarto Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>ECR</t>
+  </si>
+  <si>
+    <t>JHC</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>Equipo DNIA</t>
+  </si>
+  <si>
+    <t>ECMR</t>
+  </si>
+  <si>
+    <t>MdeSA-I</t>
+  </si>
+  <si>
+    <t>FAM</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>CDAM</t>
+  </si>
+  <si>
+    <t>Decano Facultad de Ciencias Exactas y Naturales</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>KLB</t>
+  </si>
+  <si>
+    <t>Directora Departamento de Matemáticas</t>
+  </si>
+  <si>
+    <t>JAFF</t>
+  </si>
+  <si>
+    <t>Director Académico Sede Palmira</t>
+  </si>
+  <si>
+    <t>TPL</t>
+  </si>
+  <si>
+    <t>JCMR</t>
+  </si>
+  <si>
+    <t>Sede Amazonía</t>
+  </si>
+  <si>
+    <t>AmzSP-I</t>
+  </si>
+  <si>
+    <t>GIO</t>
+  </si>
+  <si>
+    <t>HACM</t>
+  </si>
+  <si>
+    <t>JGCR</t>
+  </si>
+  <si>
+    <t>AMMH</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>PAP</t>
+  </si>
+  <si>
+    <t>JG</t>
+  </si>
+  <si>
+    <t>JDOC</t>
+  </si>
+  <si>
+    <t>Sede Caribe</t>
+  </si>
+  <si>
+    <t>CrbSP-I</t>
+  </si>
+  <si>
+    <t>AIOM</t>
+  </si>
+  <si>
+    <t>Sede Orinoquía</t>
+  </si>
+  <si>
+    <t>OrnSP-I</t>
+  </si>
+  <si>
+    <t>JFGR</t>
+  </si>
+  <si>
+    <t>BogSA-II</t>
+  </si>
+  <si>
+    <t>CDVS</t>
+  </si>
+  <si>
+    <t>DCP</t>
+  </si>
+  <si>
+    <t>JFR</t>
+  </si>
+  <si>
+    <t>AmzSP-II</t>
+  </si>
+  <si>
+    <t>CIA</t>
+  </si>
+  <si>
+    <t>JAM</t>
+  </si>
+  <si>
+    <t>VAL</t>
+  </si>
+  <si>
+    <t>NCO</t>
+  </si>
+  <si>
+    <t>Asistente administrativa DNIA</t>
+  </si>
+  <si>
+    <t>BogSA-V</t>
+  </si>
+  <si>
+    <t>AGRG</t>
+  </si>
+  <si>
+    <t>JPT</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>VSC</t>
+  </si>
+  <si>
+    <t>KMMO</t>
+  </si>
+  <si>
+    <t>Coordinadora funcional Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>LFM</t>
+  </si>
+  <si>
+    <t>Diseñadora visual Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>Asesora Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>Extensionista Facultad de Ciencias Exactas y Naturales</t>
+  </si>
+  <si>
+    <t>VJMS</t>
+  </si>
+  <si>
+    <t>AmzSP-V</t>
+  </si>
+  <si>
+    <t>LMPM</t>
+  </si>
+  <si>
+    <t>Líder pedagógica</t>
+  </si>
+  <si>
+    <t>SEBA</t>
+  </si>
+  <si>
+    <t>Líder de psicología</t>
+  </si>
+  <si>
+    <t>IVRC</t>
+  </si>
+  <si>
+    <t>JESB</t>
+  </si>
+  <si>
+    <t>Quinto Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>MLRB</t>
+  </si>
+  <si>
+    <t>Directora Departamento de Comunicación Humana Facultad de Medicina</t>
+  </si>
+  <si>
+    <t>AFOA</t>
+  </si>
+  <si>
+    <t>Director CEMarin</t>
+  </si>
+  <si>
+    <t>ASM</t>
+  </si>
+  <si>
+    <t>Directora Sede Caribe</t>
+  </si>
+  <si>
+    <t>DASC</t>
+  </si>
+  <si>
+    <t>AAD</t>
+  </si>
+  <si>
+    <t>RVM</t>
+  </si>
+  <si>
+    <t>Grupo de investigación TecMarín</t>
+  </si>
+  <si>
+    <t>LMEO</t>
+  </si>
+  <si>
+    <t>JAB</t>
+  </si>
+  <si>
+    <t>SVO</t>
+  </si>
+  <si>
+    <t>Maestría en Políticas Públicas</t>
+  </si>
+  <si>
+    <t>PVS</t>
+  </si>
+  <si>
+    <t>CrbSP-II</t>
+  </si>
+  <si>
+    <t>SCM</t>
+  </si>
+  <si>
+    <t>ELB</t>
+  </si>
+  <si>
+    <t>BBC</t>
+  </si>
+  <si>
+    <t>CrbSP-III</t>
+  </si>
+  <si>
+    <t>NDG</t>
+  </si>
+  <si>
+    <t>KBG</t>
+  </si>
+  <si>
+    <t>Artista raizal, participante proyecto El Otro Mar</t>
+  </si>
+  <si>
+    <t>CrbSP-IV</t>
+  </si>
+  <si>
+    <t>QBG</t>
+  </si>
+  <si>
+    <t>Funcionario Corporación para el Desarrollo Sostenible del Archipiélago de San Andrés</t>
+  </si>
+  <si>
+    <t>GMS</t>
+  </si>
+  <si>
+    <t>Funcionario Gobernación de San Andrés</t>
+  </si>
+  <si>
+    <t>KJR</t>
+  </si>
+  <si>
+    <t>LAH</t>
+  </si>
+  <si>
+    <t>LFS</t>
+  </si>
+  <si>
+    <t>CCB</t>
+  </si>
+  <si>
+    <t>CMG</t>
+  </si>
+  <si>
+    <t>PalSA-IV</t>
+  </si>
+  <si>
+    <t>EEF</t>
+  </si>
+  <si>
+    <t>Extensión Sede Caribe</t>
+  </si>
+  <si>
+    <t>CrbSP-V</t>
+  </si>
+  <si>
+    <t>FGP</t>
+  </si>
+  <si>
+    <t>Coordinadora de la Unidad de Transformación Pedagógica</t>
+  </si>
+  <si>
+    <t>Sexto Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>GAAG</t>
+  </si>
+  <si>
+    <t>JFRA</t>
+  </si>
+  <si>
+    <t>Maestría en Estudios Amazónicos</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>Dirección Académica</t>
+  </si>
+  <si>
+    <t>HZA</t>
+  </si>
+  <si>
+    <t>AMGC</t>
+  </si>
+  <si>
+    <t>Unidad de Transformación Pedagógica</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>DLMG</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>CJQC</t>
+  </si>
+  <si>
+    <t>JPR</t>
+  </si>
+  <si>
+    <t>LQ</t>
+  </si>
+  <si>
+    <t>ALRT</t>
+  </si>
+  <si>
+    <t>Grupo de Apoyo Pedagógico Facultad de Medicina</t>
+  </si>
+  <si>
+    <t>JCGN</t>
+  </si>
+  <si>
+    <t>Integrante Instituto de Estudios en Comunicación y Cultura (IECO)</t>
+  </si>
+  <si>
+    <t>MABU</t>
+  </si>
+  <si>
+    <t>PEAMA Orinoquía (Sede origen)</t>
+  </si>
+  <si>
+    <t>LMMV</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>Centro Latinoamericano de Investigación e Innovación Científica (CLIIC)</t>
+  </si>
+  <si>
+    <t>BogSA-VII</t>
+  </si>
+  <si>
+    <t>SLPH</t>
+  </si>
+  <si>
+    <t>EAR</t>
+  </si>
+  <si>
+    <t>MAVP</t>
+  </si>
+  <si>
+    <t>Administrativo</t>
+  </si>
+  <si>
+    <t>Supernumeraria</t>
+  </si>
+  <si>
+    <t>CrbSP-VI</t>
+  </si>
+  <si>
+    <t>Sede De La Paz</t>
+  </si>
+  <si>
+    <t>JAO</t>
+  </si>
+  <si>
+    <t>Intérprete Lengua de Señas Colombiana</t>
+  </si>
+  <si>
+    <t>YAG</t>
+  </si>
+  <si>
+    <t>WAAC</t>
+  </si>
+  <si>
+    <t>DGH</t>
+  </si>
+  <si>
+    <t>Proyecto Política de Educación Inclusiva UNAL</t>
+  </si>
+  <si>
+    <t>AMC</t>
+  </si>
+  <si>
+    <t>Profesional de apoyo Política de Educación Inclusiva</t>
+  </si>
+  <si>
+    <t>JCRB</t>
+  </si>
+  <si>
+    <t>Coordinador Acompañamiento Integral Bienestar Universitario</t>
+  </si>
+  <si>
+    <t>SBD</t>
+  </si>
+  <si>
+    <t>Diseño web Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>Sistematización de datos Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>RARR</t>
+  </si>
+  <si>
+    <t>Directora Bienestar Universitario Sede Manizales y Directora del proyecto Política de Educación Inclusiva UNAL</t>
+  </si>
+  <si>
+    <t>NGG</t>
+  </si>
+  <si>
+    <t>Vicerrector Sede Manizales</t>
+  </si>
+  <si>
+    <t>CSLMR</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>PEAMA Tumaco (Sede Origen)</t>
+  </si>
+  <si>
+    <t>REOB</t>
+  </si>
+  <si>
+    <t>JSAH</t>
+  </si>
+  <si>
+    <t>Representante Estudiantil Consejo Académico</t>
+  </si>
+  <si>
+    <t>FAMJ</t>
+  </si>
+  <si>
+    <t>RHPS</t>
+  </si>
+  <si>
+    <t>KAPJ</t>
+  </si>
+  <si>
+    <t>PEAMA Amazonía (Sede Origen)</t>
+  </si>
+  <si>
+    <t>MdeSA-II</t>
+  </si>
+  <si>
+    <t>ICRS</t>
+  </si>
+  <si>
+    <t>Sistema de Acompañamiento Estudiantil Bienestar Universitario</t>
+  </si>
+  <si>
+    <t>PalSA-V</t>
+  </si>
+  <si>
+    <t>MACA</t>
+  </si>
+  <si>
+    <t>PEAMA Caribe (Sede Origen)</t>
+  </si>
+  <si>
+    <t>PalSA-II</t>
+  </si>
+  <si>
+    <t>JDHM</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>Sin identificar</t>
+  </si>
+  <si>
+    <t>NA-VII</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>Séptimo Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>CRVM</t>
+  </si>
+  <si>
+    <t>Integrante Colectivo Cuerpos diversos en rebeldía</t>
+  </si>
+  <si>
+    <t>LEMA</t>
+  </si>
+  <si>
+    <t>EAER</t>
+  </si>
+  <si>
+    <t>KBV</t>
+  </si>
+  <si>
+    <t>Integrante Colectivo Cuerpos diversos en rebeldía
 PEAMA Orinoquía (Sede Origen)</t>
   </si>
   <si>
-    <t xml:space="preserve">JABG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCMC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OrnSP-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAPG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OMAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MFAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSZJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LCJC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KAML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCMH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMAQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VLG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestor cultural municipio de Arauca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OrnSP-IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KGC</t>
+    <t>JABG</t>
+  </si>
+  <si>
+    <t>MCMC</t>
+  </si>
+  <si>
+    <t>WSR</t>
+  </si>
+  <si>
+    <t>OrnSP-II</t>
+  </si>
+  <si>
+    <t>BAPG</t>
+  </si>
+  <si>
+    <t>OMAC</t>
+  </si>
+  <si>
+    <t>MFAC</t>
+  </si>
+  <si>
+    <t>SRM</t>
+  </si>
+  <si>
+    <t>RSZJ</t>
+  </si>
+  <si>
+    <t>LCJC</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>KAML</t>
+  </si>
+  <si>
+    <t>JCMH</t>
+  </si>
+  <si>
+    <t>SMAQ</t>
+  </si>
+  <si>
+    <t>VLG</t>
+  </si>
+  <si>
+    <t>JCT</t>
+  </si>
+  <si>
+    <t>Gestor cultural municipio de Arauca</t>
+  </si>
+  <si>
+    <t>OrnSP-IV</t>
+  </si>
+  <si>
+    <t>KGC</t>
   </si>
   <si>
     <t xml:space="preserve">Bienestar Universitario </t>
   </si>
   <si>
-    <t xml:space="preserve">OrnSP-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MJMC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LRP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profesional Universitario Informática</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OrnSP-VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JJPP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RDTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institución Educativa Bellas Artes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KFR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMRV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bienestar Universitario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TmcSP-VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Octavo Encuentro Intersedes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vicerrector General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecosistema de Innovación Académica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JJS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Director Sede Tumaco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FABZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCMO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integrante Huerta Comunitaria Nâksí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WBG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colectivo ForMa Mediación Cultural</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asesora Producción audiovisual Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LPVT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TmcSP-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DYOQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bienestar Universitario Sede Tumaco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAGV</t>
+    <t>OrnSP-V</t>
+  </si>
+  <si>
+    <t>MJMC</t>
+  </si>
+  <si>
+    <t>LRP</t>
+  </si>
+  <si>
+    <t>JCO</t>
+  </si>
+  <si>
+    <t>Profesional Universitario Informática</t>
+  </si>
+  <si>
+    <t>OrnSP-VI</t>
+  </si>
+  <si>
+    <t>JJPP</t>
+  </si>
+  <si>
+    <t>RDTE</t>
+  </si>
+  <si>
+    <t>Institución Educativa Bellas Artes</t>
+  </si>
+  <si>
+    <t>KFR</t>
+  </si>
+  <si>
+    <t>LMRV</t>
+  </si>
+  <si>
+    <t>Bienestar Universitario</t>
+  </si>
+  <si>
+    <t>TmcSP-VI</t>
+  </si>
+  <si>
+    <t>Octavo Encuentro Intersedes</t>
+  </si>
+  <si>
+    <t>Vicerrector General</t>
+  </si>
+  <si>
+    <t>Ecosistema de Innovación Académica</t>
+  </si>
+  <si>
+    <t>OEL</t>
+  </si>
+  <si>
+    <t>MAHS</t>
+  </si>
+  <si>
+    <t>AIMP</t>
+  </si>
+  <si>
+    <t>JJS</t>
+  </si>
+  <si>
+    <t>Director Sede Tumaco</t>
+  </si>
+  <si>
+    <t>FABZ</t>
+  </si>
+  <si>
+    <t>JCMO</t>
+  </si>
+  <si>
+    <t>Integrante Huerta Comunitaria Nâksí</t>
+  </si>
+  <si>
+    <t>WBG</t>
+  </si>
+  <si>
+    <t>Colectivo ForMa Mediación Cultural</t>
+  </si>
+  <si>
+    <t>LSH</t>
+  </si>
+  <si>
+    <t>Asesora Producción audiovisual Proyecto Instituto Nacional de Investigación, Innovación y Política Educativa</t>
+  </si>
+  <si>
+    <t>LPVT</t>
+  </si>
+  <si>
+    <t>TmcSP-V</t>
+  </si>
+  <si>
+    <t>DYOQ</t>
+  </si>
+  <si>
+    <t>Bienestar Universitario Sede Tumaco</t>
+  </si>
+  <si>
+    <t>DAGV</t>
+  </si>
+  <si>
+    <t>N.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -951,22 +956,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Ancizar Sans"/>
@@ -981,7 +971,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Ancizar Sans"/>
@@ -989,7 +979,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1006,161 +996,119 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1192,7 +1140,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1216,7 +1164,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1276,37 +1224,38 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H249"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K249"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B249" activeCellId="0" sqref="B249"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="26.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="22.11"/>
+    <col min="1" max="2" width="26.36328125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" customWidth="1"/>
+    <col min="7" max="8" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:11" ht="26">
+      <c r="A1" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1329,8 +1278,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+    <row r="2" spans="1:11">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1355,8 +1304,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+    <row r="3" spans="1:11" ht="37.5">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1381,8 +1330,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:11" ht="50">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1407,8 +1356,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+    <row r="5" spans="1:11" ht="37.5">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1433,8 +1382,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+    <row r="6" spans="1:11">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1459,8 +1408,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="52.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+    <row r="7" spans="1:11" ht="50">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1484,9 +1433,10 @@
       <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1511,8 +1461,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+    <row r="9" spans="1:11" ht="25">
+      <c r="A9" s="2">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1537,8 +1487,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+    <row r="10" spans="1:11">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1563,8 +1513,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
+    <row r="11" spans="1:11" ht="25">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1589,8 +1539,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
+    <row r="12" spans="1:11">
+      <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1615,8 +1565,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+    <row r="13" spans="1:11" ht="37.5">
+      <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1641,8 +1591,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+    <row r="14" spans="1:11">
+      <c r="A14" s="2">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1667,8 +1617,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
+    <row r="15" spans="1:11" ht="50">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1693,8 +1643,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
+    <row r="16" spans="1:11">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1719,8 +1669,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
+    <row r="17" spans="1:8">
+      <c r="A17" s="2">
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1745,8 +1695,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
+    <row r="18" spans="1:8" ht="25">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1771,8 +1721,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
+    <row r="19" spans="1:8" ht="50">
+      <c r="A19" s="2">
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1797,8 +1747,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+    <row r="20" spans="1:8">
+      <c r="A20" s="2">
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1823,8 +1773,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+    <row r="21" spans="1:8" ht="37.5">
+      <c r="A21" s="2">
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1849,8 +1799,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="n">
+    <row r="22" spans="1:8" ht="50">
+      <c r="A22" s="2">
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1875,8 +1825,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
+    <row r="23" spans="1:8" ht="37.5">
+      <c r="A23" s="2">
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1901,8 +1851,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
+    <row r="24" spans="1:8">
+      <c r="A24" s="2">
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1927,8 +1877,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="n">
+    <row r="25" spans="1:8">
+      <c r="A25" s="2">
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1953,8 +1903,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="n">
+    <row r="26" spans="1:8" ht="50">
+      <c r="A26" s="2">
         <v>3</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1979,8 +1929,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="n">
+    <row r="27" spans="1:8">
+      <c r="A27" s="2">
         <v>3</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2005,8 +1955,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="n">
+    <row r="28" spans="1:8" ht="38.5">
+      <c r="A28" s="2">
         <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2031,8 +1981,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="n">
+    <row r="29" spans="1:8">
+      <c r="A29" s="2">
         <v>3</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2057,8 +2007,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="n">
+    <row r="30" spans="1:8">
+      <c r="A30" s="2">
         <v>3</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2083,8 +2033,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="n">
+    <row r="31" spans="1:8">
+      <c r="A31" s="2">
         <v>3</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2109,8 +2059,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="n">
+    <row r="32" spans="1:8">
+      <c r="A32" s="2">
         <v>3</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2135,8 +2085,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="n">
+    <row r="33" spans="1:8" ht="25">
+      <c r="A33" s="2">
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2161,8 +2111,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="n">
+    <row r="34" spans="1:8" ht="62.5">
+      <c r="A34" s="2">
         <v>3</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2187,8 +2137,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="n">
+    <row r="35" spans="1:8" ht="50">
+      <c r="A35" s="2">
         <v>3</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2213,8 +2163,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="n">
+    <row r="36" spans="1:8">
+      <c r="A36" s="2">
         <v>4</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2239,8 +2189,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="n">
+    <row r="37" spans="1:8" ht="37.5">
+      <c r="A37" s="2">
         <v>4</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -2265,8 +2215,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="n">
+    <row r="38" spans="1:8" ht="50">
+      <c r="A38" s="2">
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2291,8 +2241,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="n">
+    <row r="39" spans="1:8" ht="37.5">
+      <c r="A39" s="2">
         <v>4</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -2317,8 +2267,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="n">
+    <row r="40" spans="1:8">
+      <c r="A40" s="2">
         <v>4</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2343,8 +2293,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="n">
+    <row r="41" spans="1:8">
+      <c r="A41" s="2">
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2369,8 +2319,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="n">
+    <row r="42" spans="1:8">
+      <c r="A42" s="2">
         <v>4</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -2395,8 +2345,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="n">
+    <row r="43" spans="1:8">
+      <c r="A43" s="2">
         <v>4</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2421,8 +2371,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="n">
+    <row r="44" spans="1:8" ht="50">
+      <c r="A44" s="2">
         <v>4</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2447,8 +2397,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="n">
+    <row r="45" spans="1:8">
+      <c r="A45" s="2">
         <v>4</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -2473,8 +2423,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="n">
+    <row r="46" spans="1:8" ht="37.5">
+      <c r="A46" s="2">
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2499,8 +2449,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="2" t="n">
+    <row r="47" spans="1:8">
+      <c r="A47" s="2">
         <v>4</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2525,8 +2475,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="n">
+    <row r="48" spans="1:8" ht="25">
+      <c r="A48" s="2">
         <v>4</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2551,8 +2501,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="n">
+    <row r="49" spans="1:8">
+      <c r="A49" s="2">
         <v>4</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2577,8 +2527,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="n">
+    <row r="50" spans="1:8" ht="25">
+      <c r="A50" s="2">
         <v>4</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2603,8 +2553,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="n">
+    <row r="51" spans="1:8">
+      <c r="A51" s="2">
         <v>4</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2629,8 +2579,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="n">
+    <row r="52" spans="1:8" ht="25">
+      <c r="A52" s="2">
         <v>4</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2655,8 +2605,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="n">
+    <row r="53" spans="1:8" ht="25">
+      <c r="A53" s="2">
         <v>4</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -2681,8 +2631,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="n">
+    <row r="54" spans="1:8" ht="25">
+      <c r="A54" s="2">
         <v>4</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -2707,8 +2657,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="n">
+    <row r="55" spans="1:8" ht="25">
+      <c r="A55" s="2">
         <v>4</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -2733,8 +2683,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="2" t="n">
+    <row r="56" spans="1:8" ht="25">
+      <c r="A56" s="2">
         <v>4</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2759,8 +2709,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="n">
+    <row r="57" spans="1:8" ht="25">
+      <c r="A57" s="2">
         <v>4</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2785,8 +2735,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="2" t="n">
+    <row r="58" spans="1:8" ht="25">
+      <c r="A58" s="2">
         <v>4</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -2811,8 +2761,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="n">
+    <row r="59" spans="1:8" ht="25">
+      <c r="A59" s="2">
         <v>4</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -2837,8 +2787,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="2" t="n">
+    <row r="60" spans="1:8" ht="25">
+      <c r="A60" s="2">
         <v>4</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -2863,8 +2813,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="n">
+    <row r="61" spans="1:8" ht="25">
+      <c r="A61" s="2">
         <v>4</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -2889,8 +2839,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="n">
+    <row r="62" spans="1:8" ht="25">
+      <c r="A62" s="2">
         <v>4</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2915,8 +2865,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="2" t="n">
+    <row r="63" spans="1:8">
+      <c r="A63" s="2">
         <v>4</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -2941,8 +2891,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="n">
+    <row r="64" spans="1:8">
+      <c r="A64" s="2">
         <v>4</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -2967,8 +2917,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="n">
+    <row r="65" spans="1:8">
+      <c r="A65" s="2">
         <v>4</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -2993,8 +2943,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="n">
+    <row r="66" spans="1:8" ht="38.5">
+      <c r="A66" s="2">
         <v>4</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -3019,8 +2969,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="n">
+    <row r="67" spans="1:8" ht="25">
+      <c r="A67" s="2">
         <v>4</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -3045,8 +2995,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2" t="n">
+    <row r="68" spans="1:8" ht="25">
+      <c r="A68" s="2">
         <v>4</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -3071,8 +3021,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="n">
+    <row r="69" spans="1:8" ht="25">
+      <c r="A69" s="2">
         <v>4</v>
       </c>
       <c r="B69" s="2" t="s">
@@ -3097,8 +3047,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="n">
+    <row r="70" spans="1:8" ht="25">
+      <c r="A70" s="2">
         <v>4</v>
       </c>
       <c r="B70" s="2" t="s">
@@ -3123,8 +3073,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="n">
+    <row r="71" spans="1:8" ht="25">
+      <c r="A71" s="2">
         <v>4</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -3149,8 +3099,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="n">
+    <row r="72" spans="1:8">
+      <c r="A72" s="2">
         <v>4</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -3175,8 +3125,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="n">
+    <row r="73" spans="1:8">
+      <c r="A73" s="2">
         <v>4</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -3201,8 +3151,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="n">
+    <row r="74" spans="1:8">
+      <c r="A74" s="2">
         <v>4</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -3227,8 +3177,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="n">
+    <row r="75" spans="1:8">
+      <c r="A75" s="2">
         <v>4</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -3253,8 +3203,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="n">
+    <row r="76" spans="1:8" ht="50">
+      <c r="A76" s="2">
         <v>4</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -3279,8 +3229,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="2" t="n">
+    <row r="77" spans="1:8" ht="62.5">
+      <c r="A77" s="2">
         <v>4</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -3305,8 +3255,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="2" t="n">
+    <row r="78" spans="1:8" ht="62.5">
+      <c r="A78" s="2">
         <v>4</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -3331,8 +3281,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="n">
+    <row r="79" spans="1:8" ht="50">
+      <c r="A79" s="2">
         <v>4</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -3357,8 +3307,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="2" t="n">
+    <row r="80" spans="1:8" ht="37.5">
+      <c r="A80" s="2">
         <v>4</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -3383,8 +3333,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="2" t="n">
+    <row r="81" spans="1:8" ht="25">
+      <c r="A81" s="2">
         <v>4</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -3409,8 +3359,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="2" t="n">
+    <row r="82" spans="1:8" ht="25">
+      <c r="A82" s="2">
         <v>4</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -3435,8 +3385,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="n">
+    <row r="83" spans="1:8" ht="25">
+      <c r="A83" s="2">
         <v>4</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -3461,8 +3411,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="n">
+    <row r="84" spans="1:8" ht="25">
+      <c r="A84" s="2">
         <v>4</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -3487,8 +3437,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="n">
+    <row r="85" spans="1:8" ht="25">
+      <c r="A85" s="2">
         <v>4</v>
       </c>
       <c r="B85" s="2" t="s">
@@ -3513,8 +3463,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="n">
+    <row r="86" spans="1:8" ht="37.5">
+      <c r="A86" s="2">
         <v>5</v>
       </c>
       <c r="B86" s="2" t="s">
@@ -3539,8 +3489,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="n">
+    <row r="87" spans="1:8" ht="37.5">
+      <c r="A87" s="2">
         <v>5</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -3565,8 +3515,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="2" t="n">
+    <row r="88" spans="1:8" ht="50">
+      <c r="A88" s="2">
         <v>5</v>
       </c>
       <c r="B88" s="2" t="s">
@@ -3591,8 +3541,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="n">
+    <row r="89" spans="1:8" ht="37.5">
+      <c r="A89" s="2">
         <v>5</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -3617,8 +3567,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="2" t="n">
+    <row r="90" spans="1:8">
+      <c r="A90" s="2">
         <v>5</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -3643,8 +3593,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="2" t="n">
+    <row r="91" spans="1:8" ht="50">
+      <c r="A91" s="2">
         <v>5</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -3669,8 +3619,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="n">
+    <row r="92" spans="1:8">
+      <c r="A92" s="2">
         <v>5</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -3695,8 +3645,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="n">
+    <row r="93" spans="1:8" ht="25">
+      <c r="A93" s="2">
         <v>5</v>
       </c>
       <c r="B93" s="2" t="s">
@@ -3721,8 +3671,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="n">
+    <row r="94" spans="1:8" ht="25">
+      <c r="A94" s="2">
         <v>5</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -3747,8 +3697,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="2" t="n">
+    <row r="95" spans="1:8" ht="25">
+      <c r="A95" s="2">
         <v>5</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -3773,8 +3723,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="n">
+    <row r="96" spans="1:8" ht="25">
+      <c r="A96" s="2">
         <v>5</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -3799,8 +3749,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="2" t="n">
+    <row r="97" spans="1:8" ht="25">
+      <c r="A97" s="2">
         <v>5</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -3825,8 +3775,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="n">
+    <row r="98" spans="1:8" ht="25">
+      <c r="A98" s="2">
         <v>5</v>
       </c>
       <c r="B98" s="2" t="s">
@@ -3851,8 +3801,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="n">
+    <row r="99" spans="1:8" ht="25">
+      <c r="A99" s="2">
         <v>5</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -3877,8 +3827,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="n">
+    <row r="100" spans="1:8" ht="25">
+      <c r="A100" s="2">
         <v>5</v>
       </c>
       <c r="B100" s="2" t="s">
@@ -3903,8 +3853,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="n">
+    <row r="101" spans="1:8" ht="25">
+      <c r="A101" s="2">
         <v>5</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -3929,8 +3879,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="n">
+    <row r="102" spans="1:8" ht="25">
+      <c r="A102" s="2">
         <v>5</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -3955,8 +3905,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="n">
+    <row r="103" spans="1:8" ht="25">
+      <c r="A103" s="2">
         <v>5</v>
       </c>
       <c r="B103" s="2" t="s">
@@ -3981,8 +3931,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="n">
+    <row r="104" spans="1:8" ht="25">
+      <c r="A104" s="2">
         <v>5</v>
       </c>
       <c r="B104" s="2" t="s">
@@ -4007,8 +3957,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="2" t="n">
+    <row r="105" spans="1:8" ht="25">
+      <c r="A105" s="2">
         <v>5</v>
       </c>
       <c r="B105" s="2" t="s">
@@ -4033,8 +3983,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="2" t="n">
+    <row r="106" spans="1:8" ht="25">
+      <c r="A106" s="2">
         <v>5</v>
       </c>
       <c r="B106" s="2" t="s">
@@ -4059,8 +4009,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="2" t="n">
+    <row r="107" spans="1:8" ht="25">
+      <c r="A107" s="2">
         <v>5</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -4085,8 +4035,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="2" t="n">
+    <row r="108" spans="1:8" ht="25">
+      <c r="A108" s="2">
         <v>5</v>
       </c>
       <c r="B108" s="2" t="s">
@@ -4111,8 +4061,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="2" t="n">
+    <row r="109" spans="1:8" ht="62.5">
+      <c r="A109" s="2">
         <v>5</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -4137,8 +4087,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="2" t="n">
+    <row r="110" spans="1:8" ht="25">
+      <c r="A110" s="2">
         <v>5</v>
       </c>
       <c r="B110" s="2" t="s">
@@ -4163,8 +4113,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2" t="n">
+    <row r="111" spans="1:8" ht="25">
+      <c r="A111" s="2">
         <v>5</v>
       </c>
       <c r="B111" s="2" t="s">
@@ -4189,8 +4139,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="2" t="n">
+    <row r="112" spans="1:8" ht="62.5">
+      <c r="A112" s="2">
         <v>5</v>
       </c>
       <c r="B112" s="2" t="s">
@@ -4215,8 +4165,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="2" t="n">
+    <row r="113" spans="1:8" ht="25">
+      <c r="A113" s="2">
         <v>5</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -4241,8 +4191,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="2" t="n">
+    <row r="114" spans="1:8" ht="25">
+      <c r="A114" s="2">
         <v>5</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -4267,8 +4217,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="2" t="n">
+    <row r="115" spans="1:8">
+      <c r="A115" s="2">
         <v>5</v>
       </c>
       <c r="B115" s="2" t="s">
@@ -4293,8 +4243,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="2" t="n">
+    <row r="116" spans="1:8" ht="25">
+      <c r="A116" s="2">
         <v>5</v>
       </c>
       <c r="B116" s="2" t="s">
@@ -4319,8 +4269,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="2" t="n">
+    <row r="117" spans="1:8" ht="37.5">
+      <c r="A117" s="2">
         <v>5</v>
       </c>
       <c r="B117" s="2" t="s">
@@ -4345,8 +4295,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="n">
+    <row r="118" spans="1:8" ht="62.5">
+      <c r="A118" s="2">
         <v>5</v>
       </c>
       <c r="B118" s="2" t="s">
@@ -4371,8 +4321,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="2" t="n">
+    <row r="119" spans="1:8" ht="62.5">
+      <c r="A119" s="2">
         <v>5</v>
       </c>
       <c r="B119" s="2" t="s">
@@ -4397,8 +4347,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="2" t="n">
+    <row r="120" spans="1:8" ht="25">
+      <c r="A120" s="2">
         <v>6</v>
       </c>
       <c r="B120" s="2" t="s">
@@ -4423,8 +4373,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2" t="n">
+    <row r="121" spans="1:8" ht="25">
+      <c r="A121" s="2">
         <v>6</v>
       </c>
       <c r="B121" s="2" t="s">
@@ -4449,8 +4399,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="2" t="n">
+    <row r="122" spans="1:8" ht="25">
+      <c r="A122" s="2">
         <v>6</v>
       </c>
       <c r="B122" s="2" t="s">
@@ -4475,8 +4425,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2" t="n">
+    <row r="123" spans="1:8" ht="25">
+      <c r="A123" s="2">
         <v>6</v>
       </c>
       <c r="B123" s="2" t="s">
@@ -4501,8 +4451,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2" t="n">
+    <row r="124" spans="1:8" ht="37.5">
+      <c r="A124" s="2">
         <v>6</v>
       </c>
       <c r="B124" s="2" t="s">
@@ -4527,8 +4477,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="2" t="n">
+    <row r="125" spans="1:8">
+      <c r="A125" s="2">
         <v>6</v>
       </c>
       <c r="B125" s="2" t="s">
@@ -4553,8 +4503,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="2" t="n">
+    <row r="126" spans="1:8">
+      <c r="A126" s="2">
         <v>6</v>
       </c>
       <c r="B126" s="2" t="s">
@@ -4579,8 +4529,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="2" t="n">
+    <row r="127" spans="1:8" ht="25">
+      <c r="A127" s="2">
         <v>6</v>
       </c>
       <c r="B127" s="2" t="s">
@@ -4605,8 +4555,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="2" t="n">
+    <row r="128" spans="1:8" ht="25">
+      <c r="A128" s="2">
         <v>6</v>
       </c>
       <c r="B128" s="2" t="s">
@@ -4631,8 +4581,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="2" t="n">
+    <row r="129" spans="1:8" ht="25">
+      <c r="A129" s="2">
         <v>6</v>
       </c>
       <c r="B129" s="2" t="s">
@@ -4657,8 +4607,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="2" t="n">
+    <row r="130" spans="1:8" ht="25">
+      <c r="A130" s="2">
         <v>6</v>
       </c>
       <c r="B130" s="2" t="s">
@@ -4683,8 +4633,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="2" t="n">
+    <row r="131" spans="1:8" ht="25">
+      <c r="A131" s="2">
         <v>6</v>
       </c>
       <c r="B131" s="2" t="s">
@@ -4709,8 +4659,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="2" t="n">
+    <row r="132" spans="1:8">
+      <c r="A132" s="2">
         <v>6</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -4735,8 +4685,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2" t="n">
+    <row r="133" spans="1:8">
+      <c r="A133" s="2">
         <v>6</v>
       </c>
       <c r="B133" s="2" t="s">
@@ -4761,8 +4711,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="2" t="n">
+    <row r="134" spans="1:8">
+      <c r="A134" s="2">
         <v>6</v>
       </c>
       <c r="B134" s="2" t="s">
@@ -4787,8 +4737,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="2" t="n">
+    <row r="135" spans="1:8">
+      <c r="A135" s="2">
         <v>6</v>
       </c>
       <c r="B135" s="2" t="s">
@@ -4813,8 +4763,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="2" t="n">
+    <row r="136" spans="1:8" ht="37.5">
+      <c r="A136" s="2">
         <v>6</v>
       </c>
       <c r="B136" s="2" t="s">
@@ -4839,8 +4789,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="2" t="n">
+    <row r="137" spans="1:8" ht="37.5">
+      <c r="A137" s="2">
         <v>6</v>
       </c>
       <c r="B137" s="2" t="s">
@@ -4865,8 +4815,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="2" t="n">
+    <row r="138" spans="1:8" ht="37.5">
+      <c r="A138" s="2">
         <v>6</v>
       </c>
       <c r="B138" s="2" t="s">
@@ -4891,8 +4841,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="2" t="n">
+    <row r="139" spans="1:8" ht="37.5">
+      <c r="A139" s="2">
         <v>6</v>
       </c>
       <c r="B139" s="2" t="s">
@@ -4917,8 +4867,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="2" t="n">
+    <row r="140" spans="1:8" ht="37.5">
+      <c r="A140" s="2">
         <v>6</v>
       </c>
       <c r="B140" s="2" t="s">
@@ -4943,8 +4893,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="2" t="n">
+    <row r="141" spans="1:8">
+      <c r="A141" s="2">
         <v>6</v>
       </c>
       <c r="B141" s="2" t="s">
@@ -4969,8 +4919,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="2" t="n">
+    <row r="142" spans="1:8" ht="25">
+      <c r="A142" s="2">
         <v>6</v>
       </c>
       <c r="B142" s="2" t="s">
@@ -4995,8 +4945,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="2" t="n">
+    <row r="143" spans="1:8" ht="25">
+      <c r="A143" s="2">
         <v>6</v>
       </c>
       <c r="B143" s="2" t="s">
@@ -5021,8 +4971,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="2" t="n">
+    <row r="144" spans="1:8" ht="50">
+      <c r="A144" s="2">
         <v>6</v>
       </c>
       <c r="B144" s="2" t="s">
@@ -5047,8 +4997,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="2" t="n">
+    <row r="145" spans="1:8">
+      <c r="A145" s="2">
         <v>6</v>
       </c>
       <c r="B145" s="2" t="s">
@@ -5073,8 +5023,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="2" t="n">
+    <row r="146" spans="1:8">
+      <c r="A146" s="2">
         <v>6</v>
       </c>
       <c r="B146" s="2" t="s">
@@ -5099,8 +5049,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="2" t="n">
+    <row r="147" spans="1:8">
+      <c r="A147" s="2">
         <v>6</v>
       </c>
       <c r="B147" s="2" t="s">
@@ -5125,8 +5075,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="2" t="n">
+    <row r="148" spans="1:8" ht="25">
+      <c r="A148" s="2">
         <v>6</v>
       </c>
       <c r="B148" s="2" t="s">
@@ -5151,8 +5101,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="2" t="n">
+    <row r="149" spans="1:8" ht="25">
+      <c r="A149" s="2">
         <v>6</v>
       </c>
       <c r="B149" s="2" t="s">
@@ -5177,8 +5127,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="2" t="n">
+    <row r="150" spans="1:8">
+      <c r="A150" s="2">
         <v>6</v>
       </c>
       <c r="B150" s="2" t="s">
@@ -5203,8 +5153,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="2" t="n">
+    <row r="151" spans="1:8" ht="25">
+      <c r="A151" s="2">
         <v>6</v>
       </c>
       <c r="B151" s="2" t="s">
@@ -5229,8 +5179,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="2" t="n">
+    <row r="152" spans="1:8" ht="25">
+      <c r="A152" s="2">
         <v>6</v>
       </c>
       <c r="B152" s="2" t="s">
@@ -5255,8 +5205,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="2" t="n">
+    <row r="153" spans="1:8">
+      <c r="A153" s="2">
         <v>6</v>
       </c>
       <c r="B153" s="2" t="s">
@@ -5281,8 +5231,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="2" t="n">
+    <row r="154" spans="1:8" ht="25">
+      <c r="A154" s="2">
         <v>6</v>
       </c>
       <c r="B154" s="2" t="s">
@@ -5307,8 +5257,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="2" t="n">
+    <row r="155" spans="1:8" ht="25">
+      <c r="A155" s="2">
         <v>6</v>
       </c>
       <c r="B155" s="2" t="s">
@@ -5333,8 +5283,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="2" t="n">
+    <row r="156" spans="1:8" ht="37.5">
+      <c r="A156" s="2">
         <v>6</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -5359,8 +5309,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2" t="n">
+    <row r="157" spans="1:8" ht="37.5">
+      <c r="A157" s="2">
         <v>6</v>
       </c>
       <c r="B157" s="2" t="s">
@@ -5385,8 +5335,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="2" t="n">
+    <row r="158" spans="1:8" ht="62.5">
+      <c r="A158" s="2">
         <v>6</v>
       </c>
       <c r="B158" s="2" t="s">
@@ -5411,8 +5361,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="2" t="n">
+    <row r="159" spans="1:8" ht="62.5">
+      <c r="A159" s="2">
         <v>6</v>
       </c>
       <c r="B159" s="2" t="s">
@@ -5437,8 +5387,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="2" t="n">
+    <row r="160" spans="1:8" ht="50">
+      <c r="A160" s="2">
         <v>6</v>
       </c>
       <c r="B160" s="2" t="s">
@@ -5463,8 +5413,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="2" t="n">
+    <row r="161" spans="1:8" ht="62.5">
+      <c r="A161" s="2">
         <v>6</v>
       </c>
       <c r="B161" s="2" t="s">
@@ -5489,8 +5439,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="2" t="n">
+    <row r="162" spans="1:8" ht="62.5">
+      <c r="A162" s="2">
         <v>6</v>
       </c>
       <c r="B162" s="2" t="s">
@@ -5515,8 +5465,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="2" t="n">
+    <row r="163" spans="1:8" ht="62.5">
+      <c r="A163" s="2">
         <v>6</v>
       </c>
       <c r="B163" s="2" t="s">
@@ -5541,8 +5491,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="2" t="n">
+    <row r="164" spans="1:8" ht="50">
+      <c r="A164" s="2">
         <v>6</v>
       </c>
       <c r="B164" s="2" t="s">
@@ -5567,8 +5517,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="2" t="n">
+    <row r="165" spans="1:8" ht="25">
+      <c r="A165" s="2">
         <v>6</v>
       </c>
       <c r="B165" s="2" t="s">
@@ -5593,8 +5543,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="2" t="n">
+    <row r="166" spans="1:8">
+      <c r="A166" s="2">
         <v>6</v>
       </c>
       <c r="B166" s="2" t="s">
@@ -5619,8 +5569,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="2" t="n">
+    <row r="167" spans="1:8" ht="38.5">
+      <c r="A167" s="2">
         <v>6</v>
       </c>
       <c r="B167" s="2" t="s">
@@ -5645,8 +5595,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="2" t="n">
+    <row r="168" spans="1:8" ht="25">
+      <c r="A168" s="2">
         <v>6</v>
       </c>
       <c r="B168" s="2" t="s">
@@ -5671,8 +5621,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="2" t="n">
+    <row r="169" spans="1:8">
+      <c r="A169" s="2">
         <v>6</v>
       </c>
       <c r="B169" s="2" t="s">
@@ -5697,8 +5647,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="2" t="n">
+    <row r="170" spans="1:8" ht="25">
+      <c r="A170" s="2">
         <v>6</v>
       </c>
       <c r="B170" s="2" t="s">
@@ -5723,8 +5673,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="2" t="n">
+    <row r="171" spans="1:8">
+      <c r="A171" s="2">
         <v>6</v>
       </c>
       <c r="B171" s="2" t="s">
@@ -5749,8 +5699,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="2" t="n">
+    <row r="172" spans="1:8">
+      <c r="A172" s="2">
         <v>6</v>
       </c>
       <c r="B172" s="2" t="s">
@@ -5775,8 +5725,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="2" t="n">
+    <row r="173" spans="1:8" ht="25">
+      <c r="A173" s="2">
         <v>6</v>
       </c>
       <c r="B173" s="2" t="s">
@@ -5801,8 +5751,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="2" t="n">
+    <row r="174" spans="1:8" ht="25">
+      <c r="A174" s="2">
         <v>6</v>
       </c>
       <c r="B174" s="2" t="s">
@@ -5827,8 +5777,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="2" t="n">
+    <row r="175" spans="1:8" ht="50">
+      <c r="A175" s="2">
         <v>6</v>
       </c>
       <c r="B175" s="2" t="s">
@@ -5853,8 +5803,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="2" t="n">
+    <row r="176" spans="1:8" ht="25">
+      <c r="A176" s="2">
         <v>6</v>
       </c>
       <c r="B176" s="2" t="s">
@@ -5879,8 +5829,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2" t="n">
+    <row r="177" spans="1:8" ht="25">
+      <c r="A177" s="2">
         <v>6</v>
       </c>
       <c r="B177" s="2" t="s">
@@ -5905,8 +5855,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="2" t="n">
+    <row r="178" spans="1:8" ht="25">
+      <c r="A178" s="2">
         <v>6</v>
       </c>
       <c r="B178" s="2" t="s">
@@ -5931,8 +5881,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="2" t="n">
+    <row r="179" spans="1:8">
+      <c r="A179" s="2">
         <v>6</v>
       </c>
       <c r="B179" s="2" t="s">
@@ -5957,8 +5907,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="2" t="n">
+    <row r="180" spans="1:8">
+      <c r="A180" s="2">
         <v>6</v>
       </c>
       <c r="B180" s="2" t="s">
@@ -5983,8 +5933,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="2" t="n">
+    <row r="181" spans="1:8">
+      <c r="A181" s="2">
         <v>6</v>
       </c>
       <c r="B181" s="2" t="s">
@@ -6009,8 +5959,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="2" t="n">
+    <row r="182" spans="1:8" ht="37.5">
+      <c r="A182" s="2">
         <v>7</v>
       </c>
       <c r="B182" s="2" t="s">
@@ -6035,8 +5985,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="2" t="n">
+    <row r="183" spans="1:8" ht="50">
+      <c r="A183" s="2">
         <v>7</v>
       </c>
       <c r="B183" s="2" t="s">
@@ -6061,8 +6011,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="2" t="n">
+    <row r="184" spans="1:8" ht="37.5">
+      <c r="A184" s="2">
         <v>7</v>
       </c>
       <c r="B184" s="2" t="s">
@@ -6087,8 +6037,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="2" t="n">
+    <row r="185" spans="1:8" ht="37.5">
+      <c r="A185" s="2">
         <v>7</v>
       </c>
       <c r="B185" s="2" t="s">
@@ -6113,8 +6063,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="2" t="n">
+    <row r="186" spans="1:8" ht="37.5">
+      <c r="A186" s="2">
         <v>7</v>
       </c>
       <c r="B186" s="2" t="s">
@@ -6139,8 +6089,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="2" t="n">
+    <row r="187" spans="1:8" ht="37.5">
+      <c r="A187" s="2">
         <v>7</v>
       </c>
       <c r="B187" s="2" t="s">
@@ -6165,8 +6115,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="2" t="n">
+    <row r="188" spans="1:8" ht="62.5">
+      <c r="A188" s="2">
         <v>7</v>
       </c>
       <c r="B188" s="2" t="s">
@@ -6191,8 +6141,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="2" t="n">
+    <row r="189" spans="1:8" ht="50">
+      <c r="A189" s="2">
         <v>7</v>
       </c>
       <c r="B189" s="2" t="s">
@@ -6217,8 +6167,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="2" t="n">
+    <row r="190" spans="1:8" ht="38.5">
+      <c r="A190" s="2">
         <v>7</v>
       </c>
       <c r="B190" s="2" t="s">
@@ -6243,8 +6193,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="2" t="n">
+    <row r="191" spans="1:8" ht="50">
+      <c r="A191" s="2">
         <v>7</v>
       </c>
       <c r="B191" s="2" t="s">
@@ -6269,8 +6219,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="2" t="n">
+    <row r="192" spans="1:8" ht="62.5">
+      <c r="A192" s="2">
         <v>7</v>
       </c>
       <c r="B192" s="2" t="s">
@@ -6295,8 +6245,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="2" t="n">
+    <row r="193" spans="1:8" ht="62.5">
+      <c r="A193" s="2">
         <v>7</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -6321,8 +6271,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="2" t="n">
+    <row r="194" spans="1:8" ht="62.5">
+      <c r="A194" s="2">
         <v>7</v>
       </c>
       <c r="B194" s="2" t="s">
@@ -6347,8 +6297,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="2" t="n">
+    <row r="195" spans="1:8" ht="25">
+      <c r="A195" s="2">
         <v>7</v>
       </c>
       <c r="B195" s="2" t="s">
@@ -6373,8 +6323,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="2" t="n">
+    <row r="196" spans="1:8" ht="25">
+      <c r="A196" s="2">
         <v>7</v>
       </c>
       <c r="B196" s="2" t="s">
@@ -6399,8 +6349,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="2" t="n">
+    <row r="197" spans="1:8" ht="25">
+      <c r="A197" s="2">
         <v>7</v>
       </c>
       <c r="B197" s="2" t="s">
@@ -6425,8 +6375,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="2" t="n">
+    <row r="198" spans="1:8" ht="25">
+      <c r="A198" s="2">
         <v>7</v>
       </c>
       <c r="B198" s="2" t="s">
@@ -6451,8 +6401,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="2" t="n">
+    <row r="199" spans="1:8" ht="25">
+      <c r="A199" s="2">
         <v>7</v>
       </c>
       <c r="B199" s="2" t="s">
@@ -6477,8 +6427,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="2" t="n">
+    <row r="200" spans="1:8" ht="25">
+      <c r="A200" s="2">
         <v>7</v>
       </c>
       <c r="B200" s="2" t="s">
@@ -6503,8 +6453,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="2" t="n">
+    <row r="201" spans="1:8" ht="25">
+      <c r="A201" s="2">
         <v>7</v>
       </c>
       <c r="B201" s="2" t="s">
@@ -6529,8 +6479,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="2" t="n">
+    <row r="202" spans="1:8" ht="25">
+      <c r="A202" s="2">
         <v>7</v>
       </c>
       <c r="B202" s="2" t="s">
@@ -6555,8 +6505,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="2" t="n">
+    <row r="203" spans="1:8" ht="25">
+      <c r="A203" s="2">
         <v>7</v>
       </c>
       <c r="B203" s="2" t="s">
@@ -6581,8 +6531,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="2" t="n">
+    <row r="204" spans="1:8" ht="25">
+      <c r="A204" s="2">
         <v>7</v>
       </c>
       <c r="B204" s="2" t="s">
@@ -6607,8 +6557,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="2" t="n">
+    <row r="205" spans="1:8" ht="25">
+      <c r="A205" s="2">
         <v>7</v>
       </c>
       <c r="B205" s="2" t="s">
@@ -6633,8 +6583,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="2" t="n">
+    <row r="206" spans="1:8" ht="25">
+      <c r="A206" s="2">
         <v>7</v>
       </c>
       <c r="B206" s="2" t="s">
@@ -6659,8 +6609,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="2" t="n">
+    <row r="207" spans="1:8" ht="25">
+      <c r="A207" s="2">
         <v>7</v>
       </c>
       <c r="B207" s="2" t="s">
@@ -6685,8 +6635,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="2" t="n">
+    <row r="208" spans="1:8" ht="25">
+      <c r="A208" s="2">
         <v>7</v>
       </c>
       <c r="B208" s="2" t="s">
@@ -6711,8 +6661,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="2" t="n">
+    <row r="209" spans="1:8" ht="25">
+      <c r="A209" s="2">
         <v>7</v>
       </c>
       <c r="B209" s="2" t="s">
@@ -6737,8 +6687,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="2" t="n">
+    <row r="210" spans="1:8" ht="25">
+      <c r="A210" s="2">
         <v>7</v>
       </c>
       <c r="B210" s="2" t="s">
@@ -6763,8 +6713,8 @@
         <v>267</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="2" t="n">
+    <row r="211" spans="1:8" ht="25">
+      <c r="A211" s="2">
         <v>7</v>
       </c>
       <c r="B211" s="2" t="s">
@@ -6789,8 +6739,8 @@
         <v>270</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="2" t="n">
+    <row r="212" spans="1:8" ht="25">
+      <c r="A212" s="2">
         <v>7</v>
       </c>
       <c r="B212" s="2" t="s">
@@ -6815,8 +6765,8 @@
         <v>270</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="2" t="n">
+    <row r="213" spans="1:8" ht="25">
+      <c r="A213" s="2">
         <v>7</v>
       </c>
       <c r="B213" s="2" t="s">
@@ -6841,8 +6791,8 @@
         <v>270</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="2" t="n">
+    <row r="214" spans="1:8" ht="25">
+      <c r="A214" s="2">
         <v>7</v>
       </c>
       <c r="B214" s="2" t="s">
@@ -6867,8 +6817,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="2" t="n">
+    <row r="215" spans="1:8" ht="25">
+      <c r="A215" s="2">
         <v>7</v>
       </c>
       <c r="B215" s="2" t="s">
@@ -6893,8 +6843,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="2" t="n">
+    <row r="216" spans="1:8" ht="25">
+      <c r="A216" s="2">
         <v>7</v>
       </c>
       <c r="B216" s="2" t="s">
@@ -6919,8 +6869,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="2" t="n">
+    <row r="217" spans="1:8" ht="25">
+      <c r="A217" s="2">
         <v>7</v>
       </c>
       <c r="B217" s="2" t="s">
@@ -6945,8 +6895,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="2" t="n">
+    <row r="218" spans="1:8" ht="25">
+      <c r="A218" s="2">
         <v>7</v>
       </c>
       <c r="B218" s="2" t="s">
@@ -6971,8 +6921,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="2" t="n">
+    <row r="219" spans="1:8" ht="50">
+      <c r="A219" s="2">
         <v>7</v>
       </c>
       <c r="B219" s="2" t="s">
@@ -6997,8 +6947,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="2" t="n">
+    <row r="220" spans="1:8" ht="25">
+      <c r="A220" s="2">
         <v>7</v>
       </c>
       <c r="B220" s="2" t="s">
@@ -7023,8 +6973,8 @@
         <v>282</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="2" t="n">
+    <row r="221" spans="1:8" ht="37.5">
+      <c r="A221" s="2">
         <v>8</v>
       </c>
       <c r="B221" s="2" t="s">
@@ -7049,8 +6999,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="2" t="n">
+    <row r="222" spans="1:8">
+      <c r="A222" s="2">
         <v>8</v>
       </c>
       <c r="B222" s="2" t="s">
@@ -7075,8 +7025,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="2" t="n">
+    <row r="223" spans="1:8" ht="25">
+      <c r="A223" s="2">
         <v>8</v>
       </c>
       <c r="B223" s="2" t="s">
@@ -7101,8 +7051,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="6" t="n">
+    <row r="224" spans="1:8">
+      <c r="A224" s="6">
         <v>8</v>
       </c>
       <c r="B224" s="2" t="s">
@@ -7127,8 +7077,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="6" t="n">
+    <row r="225" spans="1:8">
+      <c r="A225" s="6">
         <v>8</v>
       </c>
       <c r="B225" s="2" t="s">
@@ -7153,8 +7103,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="6" t="n">
+    <row r="226" spans="1:8" ht="50">
+      <c r="A226" s="6">
         <v>8</v>
       </c>
       <c r="B226" s="2" t="s">
@@ -7179,8 +7129,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="6" t="n">
+    <row r="227" spans="1:8">
+      <c r="A227" s="6">
         <v>8</v>
       </c>
       <c r="B227" s="2" t="s">
@@ -7205,8 +7155,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="6" t="n">
+    <row r="228" spans="1:8">
+      <c r="A228" s="6">
         <v>8</v>
       </c>
       <c r="B228" s="2" t="s">
@@ -7231,8 +7181,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="6" t="n">
+    <row r="229" spans="1:8" ht="25">
+      <c r="A229" s="6">
         <v>8</v>
       </c>
       <c r="B229" s="2" t="s">
@@ -7257,8 +7207,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="6" t="n">
+    <row r="230" spans="1:8" ht="25">
+      <c r="A230" s="6">
         <v>8</v>
       </c>
       <c r="B230" s="2" t="s">
@@ -7283,8 +7233,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="6" t="n">
+    <row r="231" spans="1:8" ht="25">
+      <c r="A231" s="6">
         <v>8</v>
       </c>
       <c r="B231" s="2" t="s">
@@ -7309,8 +7259,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="6" t="n">
+    <row r="232" spans="1:8" ht="25">
+      <c r="A232" s="6">
         <v>8</v>
       </c>
       <c r="B232" s="2" t="s">
@@ -7335,8 +7285,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="6" t="n">
+    <row r="233" spans="1:8" ht="25">
+      <c r="A233" s="6">
         <v>8</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -7361,8 +7311,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="6" t="n">
+    <row r="234" spans="1:8" ht="25">
+      <c r="A234" s="6">
         <v>8</v>
       </c>
       <c r="B234" s="2" t="s">
@@ -7387,8 +7337,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="6" t="n">
+    <row r="235" spans="1:8" ht="25">
+      <c r="A235" s="6">
         <v>8</v>
       </c>
       <c r="B235" s="2" t="s">
@@ -7413,8 +7363,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="236" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="6" t="n">
+    <row r="236" spans="1:8">
+      <c r="A236" s="6">
         <v>8</v>
       </c>
       <c r="B236" s="2" t="s">
@@ -7439,8 +7389,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="6" t="n">
+    <row r="237" spans="1:8" ht="25">
+      <c r="A237" s="6">
         <v>8</v>
       </c>
       <c r="B237" s="2" t="s">
@@ -7465,8 +7415,8 @@
         <v>156</v>
       </c>
     </row>
-    <row r="238" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="6" t="n">
+    <row r="238" spans="1:8" ht="62.5">
+      <c r="A238" s="6">
         <v>8</v>
       </c>
       <c r="B238" s="2" t="s">
@@ -7491,8 +7441,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="2" t="n">
+    <row r="239" spans="1:8" ht="62.5">
+      <c r="A239" s="2">
         <v>8</v>
       </c>
       <c r="B239" s="2" t="s">
@@ -7517,8 +7467,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="2" t="n">
+    <row r="240" spans="1:8" ht="62.5">
+      <c r="A240" s="2">
         <v>8</v>
       </c>
       <c r="B240" s="2" t="s">
@@ -7543,8 +7493,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="2" t="n">
+    <row r="241" spans="1:8" ht="50">
+      <c r="A241" s="2">
         <v>8</v>
       </c>
       <c r="B241" s="2" t="s">
@@ -7569,8 +7519,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="2" t="n">
+    <row r="242" spans="1:8" ht="62.5">
+      <c r="A242" s="2">
         <v>8</v>
       </c>
       <c r="B242" s="2" t="s">
@@ -7595,8 +7545,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="2" t="n">
+    <row r="243" spans="1:8" ht="25">
+      <c r="A243" s="2">
         <v>8</v>
       </c>
       <c r="B243" s="2" t="s">
@@ -7621,8 +7571,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="2" t="n">
+    <row r="244" spans="1:8" ht="25">
+      <c r="A244" s="2">
         <v>8</v>
       </c>
       <c r="B244" s="2" t="s">
@@ -7647,8 +7597,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="2" t="n">
+    <row r="245" spans="1:8" ht="25">
+      <c r="A245" s="2">
         <v>8</v>
       </c>
       <c r="B245" s="2" t="s">
@@ -7673,8 +7623,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="2" t="n">
+    <row r="246" spans="1:8" ht="25">
+      <c r="A246" s="2">
         <v>8</v>
       </c>
       <c r="B246" s="2" t="s">
@@ -7699,18 +7649,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" spans="1:8">
       <c r="B249" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H246"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <autoFilter ref="A1:H246" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>